<commit_message>
Cambios de los excel e icono de usuarios
</commit_message>
<xml_diff>
--- a/public/Plantilla1.xlsx
+++ b/public/Plantilla1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\hg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,9 +50,6 @@
     <t>Periodo</t>
   </si>
   <si>
-    <t>Mecatronica</t>
-  </si>
-  <si>
     <t>ENE-MAR2023</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>No Admitidos</t>
+  </si>
+  <si>
+    <t>Sistemas</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +904,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -915,7 +915,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -937,15 +937,15 @@
         <v>11</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="2">
         <v>12</v>
@@ -967,7 +967,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>